<commit_message>
Add quiz questions for chapter 2
</commit_message>
<xml_diff>
--- a/data/quiz_questions.xlsx
+++ b/data/quiz_questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peteroehlinger/Library/CloudStorage/Dropbox/__PhD Programme/_supplyChain/intro-macro/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AK119187\Dropbox\__PhD Programme\_supplyChain\intro-macro\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BE31D5-FA12-2F4A-8C21-11827B6B30BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D17D6A-529D-4AD3-9B9C-EC33C3D6F811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{8C7F4400-6482-D949-BB12-0527E20FA512}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{8C7F4400-6482-D949-BB12-0527E20FA512}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>Question</t>
   </si>
@@ -195,6 +193,216 @@
   </si>
   <si>
     <t>Answer</t>
+  </si>
+  <si>
+    <t>Durch den Multiplikatoreffekt werden wirtschaftliche Schocks verstärkt.</t>
+  </si>
+  <si>
+    <t>Durch den Multiplikatoreffekt werden wirtschaftliche Schocks abgeschwächt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importe sind Teil des Bruttoinlandsproduktes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exporte sind Teil des Bruttoinlandsproduktes. </t>
+  </si>
+  <si>
+    <t>In unserem Gütermarktmodell werden Lagerinvestitionen nicht berücksichtigt.</t>
+  </si>
+  <si>
+    <t>In unserem Gütermarktmodell werden Lagerinvestitionen berücksichtigt.</t>
+  </si>
+  <si>
+    <t>In unserem Gütermarktmodell ignorieren wir Preisveränderungen.</t>
+  </si>
+  <si>
+    <t>Der Konsum hängt in erster Linie vom verfügbaren Einkommen ab.</t>
+  </si>
+  <si>
+    <t>Das verfügbare Einkommen ist als die Differenz zwischen Steuern und Einkommen definiert.</t>
+  </si>
+  <si>
+    <t>Das verfügbare Einkommen ist als die Differenz zwischen Einkommen und Steuern definiert.</t>
+  </si>
+  <si>
+    <t>Die marginale Konsumquote kann größer als 1 sein.</t>
+  </si>
+  <si>
+    <t>Die marginale Konsumquote kann nicht größer als 1 sein.</t>
+  </si>
+  <si>
+    <t>Entscheidungen über die Höhe der Staatsausgaben und der Steuern bezeichnet man als Fiskalpolitik.</t>
+  </si>
+  <si>
+    <t>Entscheidungen über die Höhe der Staatsausgaben und der Steuern bezeichnet man als Steuerpolitik.</t>
+  </si>
+  <si>
+    <t>Eine Variable, die von anderen Variablen abhängig ist, nennt man endogen.</t>
+  </si>
+  <si>
+    <t>Eine Variable, die nicht von den anderen Variablen eines Modells abhängt, nennt man exogen.</t>
+  </si>
+  <si>
+    <t>Eine Variable, die von anderen Variablen abhängig ist, nennt man exogen.</t>
+  </si>
+  <si>
+    <t>Eine Variable, die nicht von den anderen Variablen eines Modells abhängt, nennt man endogen.</t>
+  </si>
+  <si>
+    <t>Im Gütermarktgleichgewicht ist die Produktion von Gütern gleich der Nachfrage von Gütern.</t>
+  </si>
+  <si>
+    <t>Im Gütermarktgleichgewicht ist die Produktion von Gütern gleich dem Einkommen.</t>
+  </si>
+  <si>
+    <t>Im Gütermarktgleichgewicht sind die Investionen gleich dem öffentlichen Sparen.</t>
+  </si>
+  <si>
+    <t>Im Gütermarktgleichgewicht ist die Produktion von Gütern gleich dem Staatsausgaben.</t>
+  </si>
+  <si>
+    <t>Im Gütermarktgleichgewicht sind die Investionen gleich der gesamtwirtschaftlichen Ersparnis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einkommensabhängige Steuern verringern den Multiplikator. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einkommensabhängige Steuern erhöhen den Multiplikator. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steigt im Gütermarktmodell die marginale Konsumquote, wird die Nachfragekurve steiler. </t>
+  </si>
+  <si>
+    <t>Eine Senkung der Steuern führt im Gütermarktmodell zu einer Verschiebung der Nachfragekurve nach oben.</t>
+  </si>
+  <si>
+    <t>Eine Erhöhung der Steuern führt im Gütermarktmodell zu einer Verschiebung der Nachfragekurve nach unten.</t>
+  </si>
+  <si>
+    <t>Eine Senkung der Staatsausgaben führt im Gütermarktmodell zu einer Verschiebung der Nachfragekurve nach oben.</t>
+  </si>
+  <si>
+    <t>Eine Erhöhung der Staatsausgaben führt im Gütermarktmodell zu einer Verschiebung der Nachfragekurve nach unten.</t>
+  </si>
+  <si>
+    <t>Eine Senkung der Steuern führt im Gütermarktmodell zu einer Verschiebung der Nachfragekurve nach unten.</t>
+  </si>
+  <si>
+    <t>Eine Erhöhung der Steuern führt im Gütermarktmodell zu einer Verschiebung der Nachfragekurve nach oben.</t>
+  </si>
+  <si>
+    <t>Eine Senkung der Staatsausgaben führt im Gütermarktmodell zu einer Verschiebung der Nachfragekurve nach unten.</t>
+  </si>
+  <si>
+    <t>Eine Erhöhung der Staatsausgaben führt im Gütermarktmodell zu einer Verschiebung der Nachfragekurve nach oben.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steigt im Gütermarktmodell die marginale Konsumquote, wird die Nachfragekurve flacher. </t>
+  </si>
+  <si>
+    <t>Economic shocks are amplified by the multiplier effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Economic shocks are mitigated by the multiplier effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Imports are part of the gross domestic product</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exports are part of the gross domestic product</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In our goods market model, inventory investments are not considered</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In our goods market model, inventory investments are considered</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In our goods market model, we ignore price changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Consumption primarily depends on disposable income</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Disposable income is defined as the difference between taxes and income</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Disposable income is defined as the difference between income and taxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The marginal propensity to consume can be greater than 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The marginal propensity to consume cannot be greater than 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Decisions about the level of government spending and taxes are called fiscal policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Decisions about the level of government spending and taxes are called tax policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A variable that depends on other variables is called endogenous</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A variable that does not depend on other variables in a model is called exogenous</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A variable that depends on other variables is called exogenous</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A variable that does not depend on other variables in a model is called endogenous</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In goods market equilibrium, the production of goods equals the demand for goods</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In goods market equilibrium, the production of goods equals income</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In goods market equilibrium, the production of goods equals government spending</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In goods market equilibrium, investments equal public savings</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In goods market equilibrium, investments equal aggregate savings</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Income-dependent taxes reduce the multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Income-dependent taxes increase the multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> An increase in government spending leads to an upward shift in the demand curve in the goods market model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A decrease in government spending leads to a downward shift in the demand curve in the goods market model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> An increase in taxes leads to an upward shift in the demand curve in the goods market model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A decrease in taxes leads to a downward shift in the demand curve in the goods market model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> An increase in government spending leads to a downward shift in the demand curve in the goods market model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A decrease in government spending leads to an upward shift in the demand curve in the goods market model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> An increase in taxes leads to a downward shift in the demand curve in the goods market model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A decrease in taxes leads to an upward shift in the demand curve in the goods market model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the marginal propensity to consume rises in the goods market model, the demand curve becomes steeper</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the marginal propensity to consume rises in the goods market model, the demand curve becomes flatter.</t>
   </si>
 </sst>
 </file>
@@ -546,19 +754,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB02651-D15F-5649-AF64-9CB38539F857}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="104.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="96.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="104.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -569,7 +777,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -580,7 +788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -591,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -602,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -613,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -624,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -635,7 +843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -646,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -657,7 +865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -668,7 +876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -679,7 +887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -690,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -701,7 +909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -712,7 +920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -723,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -734,7 +942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -745,7 +953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -756,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -767,7 +975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -778,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -789,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -800,7 +1008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -811,7 +1019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -822,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -833,7 +1041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -842,6 +1050,391 @@
       </c>
       <c r="C26" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>84</v>
+      </c>
+      <c r="B54" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>81</v>
+      </c>
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>79</v>
+      </c>
+      <c r="B59" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>78</v>
+      </c>
+      <c r="B60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>87</v>
+      </c>
+      <c r="B61" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
forgot to push (I think it was mainly math equations)
</commit_message>
<xml_diff>
--- a/data/quiz_questions.xlsx
+++ b/data/quiz_questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peteroehlinger/Library/CloudStorage/Dropbox/__PhD Programme/_supplyChain/intro-macro/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF56A414-5DA7-DF45-89EB-6D1BFAE282D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7778DE5F-9346-1040-88A4-E82F2CC10AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="17520" xr2:uid="{8C7F4400-6482-D949-BB12-0527E20FA512}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{8C7F4400-6482-D949-BB12-0527E20FA512}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="285">
   <si>
     <t>Die Inflation gemessen am BIP-Deflator berücksichtigt Exporte.</t>
   </si>
@@ -403,6 +403,492 @@
   </si>
   <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>Je höher das Transaktionsvolumen, desto höher die Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Je niedriger das Transaktionsvolumen, desto niedriger die Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Je niedriger das Transaktionsvolumen, desto höher die Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Je höher das Transaktionsvolumen, desto niedriger die Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Je höher der Zinssatz desto niedriger die Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Je höher der Zinssatz desto höher die Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Je niedriger der Zinssatz desto niedriger die Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Je niedriger der Zinssatz desto höher die Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Bei gegebenem Zinssatz führt ein Anstieg des Nominaleinkommens zu einem Anstieg der Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Bei gegebenem Zinssatz führt ein Anstieg des Nominaleinkommens zu einem Rückgang der Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Bei gegebenem Zinssatz führt ein Rückgang des Nominaleinkommens zu einem Anstieg der Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Bei gegebenem Zinssatz führt ein Rückgang des Nominaleinkommens zu einem Rückgang der Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Das Hauptziel der meisten Zentralbanken ist die Preisstabilität.</t>
+  </si>
+  <si>
+    <t>Bei gegebenem Zinssatz führt ein Anstieg der Preise zu einem Anstieg der Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Bei gegebenem Zinssatz führt ein Anstieg der Preise zu einem Rückgang der Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Bei gegebenem Zinssatz führt ein Rückgang der Preise zu einem Anstieg der Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Bei gegebenem Zinssatz führt ein Rückgang der Preise zu einem Rückgang der Geldnachfrage.</t>
+  </si>
+  <si>
+    <t>Die EZB hat neben der Preisstabilität auch das Ziel der Vollbeschäftigung.</t>
+  </si>
+  <si>
+    <t>Die Fed hat neben der Preisstabilität auch das Ziel der Vollbeschäftigung.</t>
+  </si>
+  <si>
+    <t>Steigt die Inflation über das Inflationsziel hinaus, werden Zentralbanken die Zinsen eher anheben.</t>
+  </si>
+  <si>
+    <t>Steigt die Inflation über das Inflationsziel hinaus, werden Zentralbanken die Zinsen eher senken.</t>
+  </si>
+  <si>
+    <t>Zinssenkungen kurbeln das Wirtschaftswachstum an.</t>
+  </si>
+  <si>
+    <t>Zinssenkungen bremsen das Wirtschaftswachstum.</t>
+  </si>
+  <si>
+    <t>Zinserhöhungen kurbeln das Wirtschaftswachstum an.</t>
+  </si>
+  <si>
+    <t>Zinserhöhungen bremsen das Wirtschaftswachstum.</t>
+  </si>
+  <si>
+    <t>Expansive Offenmarktoperationen führen zu einer Erhöhung der Geldmenge.</t>
+  </si>
+  <si>
+    <t>Kontraktive Offenmarktoperationen führen zu einer Erhöhung der Geldmenge.</t>
+  </si>
+  <si>
+    <t>Kontraktive Offenmarktoperationen führen zu einer Reduktion der Geldmenge.</t>
+  </si>
+  <si>
+    <t>Expansive Offenmarktoperationen führen zu einer Reduktion der Geldmenge.</t>
+  </si>
+  <si>
+    <t>Verfolgt die Zentralbank eine Zinssteuerung, bleibt der Zins bei einer Erhöhung der Geldnachfrage unverändert.</t>
+  </si>
+  <si>
+    <t>Verfolgt die Zentralbank eine Zinssteuerung, bleibt die Geldmenge bei einer Erhöhung der Geldnachfrage unverändert.</t>
+  </si>
+  <si>
+    <t>Verfolgt die Zentralbank eine Geldmengensteuerung, bleibt der Zins bei einer Erhöhung der Geldnachfrage unverändert.</t>
+  </si>
+  <si>
+    <t>Verfolgt die Zentralbank eine Geldmengensteuerung, bleibt die Geldmenge bei einer Erhöhung der Geldnachfrage unverändert.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steigt die Nachfrage nach einem Wertpapier, sinkt der Preis und der Zinssatz steigt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steigt die Nachfrage nach einem Wertpapier, steigt der Preis und der Zinssatz steigt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steigt die Nachfrage nach einem Wertpapier, sinkt der Preis und der Zinssatz sinkt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steigt die Nachfrage nach einem Wertpapier, steigt der Preis und der Zinssatz sinkt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinkt die Nachfrage nach einem Wertpapier, sinkt der Preis und der Zinssatz steigt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinkt die Nachfrage nach einem Wertpapier, steigt der Preis und der Zinssatz steigt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinkt die Nachfrage nach einem Wertpapier, sinkt der Preis und der Zinssatz sinkt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinkt die Nachfrage nach einem Wertpapier, steigt der Preis und der Zinssatz sinkt. </t>
+  </si>
+  <si>
+    <t>In der Praxis verfolgen Zentralbanken meist eine Zinssteuerung.</t>
+  </si>
+  <si>
+    <t>In der Praxis verfolgen Zentralbanken meist eine Geldmengensteuerung.</t>
+  </si>
+  <si>
+    <t>The higher the transaction volume, the higher the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The higher the transaction volume, the lower the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The lower the transaction volume, the higher the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The lower the transaction volume, the lower the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The higher the interest rate, the lower the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The higher the interest rate, the higher the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The lower the interest rate, the lower the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The lower the interest rate, the higher the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> At a given interest rate, an increase in nominal income leads to an increase in the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> At a given interest rate, an increase in nominal income leads to a decrease in the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> At a given interest rate, a decrease in nominal income leads to an increase in the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> At a given interest rate, a decrease in nominal income leads to a decrease in the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> At a given interest rate, an increase in prices leads to an increase in the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> At a given interest rate, an increase in prices leads to a decrease in the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> At a given interest rate, a decrease in prices leads to an increase in the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> At a given interest rate, a decrease in prices leads to a decrease in the demand for money</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The main goal of most central banks is price stability</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The ECB has the goal of full employment in addition to price stability</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Fed has the goal of full employment in addition to price stability</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If inflation rises above the inflation target, central banks are more likely to raise interest rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If inflation rises above the inflation target, central banks are more likely to lower interest rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Interest rate cuts stimulate economic growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Interest rate cuts slow down economic growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Interest rate hikes stimulate economic growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Interest rate hikes slow down economic growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Expansionary open market operations increase the money supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Expansionary open market operations reduce the money supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Contractionary open market operations increase the money supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Contractionary open market operations reduce the money supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the central bank follows an interest rate policy, the interest rate remains unchanged when the demand for money increases</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the central bank follows an interest rate policy, the money supply remains unchanged when the demand for money increases</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the central bank follows a money supply policy, the interest rate remains unchanged when the demand for money increases</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the central bank follows a money supply policy, the money supply remains unchanged when the demand for money increases</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the demand for a security increases, the price falls, and the interest rate rises</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the demand for a security decreases, the price falls, and the interest rate rises</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the demand for a security increases, the price rises, and the interest rate rises</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the demand for a security decreases, the price rises, and the interest rate rises</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the demand for a security increases, the price falls, and the interest rate falls</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the demand for a security decreases, the price falls, and the interest rate falls</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the demand for a security increases, the price rises, and the interest rate falls</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the demand for a security decreases, the price rises, and the interest rate falls</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In practice, central banks usually follow an interest rate policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In practice, central banks usually follow a money supply policy.</t>
+  </si>
+  <si>
+    <t>Im ISLM Modell sinken die Investitionen mit steigendem Einkommen.</t>
+  </si>
+  <si>
+    <t>Im ISLM Modell steigen die Investitionen mit steigendem Einkommen.</t>
+  </si>
+  <si>
+    <t>Im ISLM Modell sinken die Investitionen mit steigendem Zins.</t>
+  </si>
+  <si>
+    <t>Im ISLM Modell steigen die Investitionen mit steigendem Zins.</t>
+  </si>
+  <si>
+    <t>Je höher die Zinssensitivität der Investitionsnachfrage, desto steiler die IS Kurve.</t>
+  </si>
+  <si>
+    <t>Je höher die Zinssensitivität der Investitionsnachfrage, desto flacher die IS Kurve.</t>
+  </si>
+  <si>
+    <t>Ein Anstieg des Zinssatzes verschiebt die Güternachfragekurve nach unten.</t>
+  </si>
+  <si>
+    <t>Ein Anstieg des Zinssatzes verschiebt die Güternachfragekurve nach oben.</t>
+  </si>
+  <si>
+    <t>Eine Reduktion des Zinssatzes verschiebt die Güternachfragekurve nach unten.</t>
+  </si>
+  <si>
+    <t>Eine Reduktion des Zinssatzes verschiebt die Güternachfragekurve nach oben.</t>
+  </si>
+  <si>
+    <t>Die IS Kurve hat einen fallenden Verlauf.</t>
+  </si>
+  <si>
+    <t>Die IS Kurve hat einen steigenden Verlauf.</t>
+  </si>
+  <si>
+    <t>Eine Erhöhung der Staatsausgaben führt zu einer Verschiebung der IS Kurve nach rechts.</t>
+  </si>
+  <si>
+    <t>Eine Erhöhung der Staatsausgaben führt zu einer Verschiebung der IS Kurve nach links.</t>
+  </si>
+  <si>
+    <t>Eine Erhöhung der Steuern führt zu einer Verschiebung der IS Kurve nach rechts.</t>
+  </si>
+  <si>
+    <t>Eine Erhöhung der Steuern führt zu einer Verschiebung der IS Kurve nach links.</t>
+  </si>
+  <si>
+    <t>Eine Senkung der Staatsausgaben führt zu einer Verschiebung der IS Kurve nach rechts.</t>
+  </si>
+  <si>
+    <t>Eine Senkung der Staatsausgaben führt zu einer Verschiebung der IS Kurve nach links.</t>
+  </si>
+  <si>
+    <t>Eine Senkung der Steuern führt zu einer Verschiebung der IS Kurve nach rechts.</t>
+  </si>
+  <si>
+    <t>Eine Senkung der Steuern führt zu einer Verschiebung der IS Kurve nach links.</t>
+  </si>
+  <si>
+    <t>Die IS Kurve beschreibt alle Kombinationen von Zins und Produktion, bei denen der Gütermarkt im Gleichgewicht ist.</t>
+  </si>
+  <si>
+    <t>Faktoren, die auf Gütermarkt bei gegebenem Zins zu einem Anstieg des Einkommens führen, verschieben die IS-Kurve nach rechts.</t>
+  </si>
+  <si>
+    <t>Faktoren, die auf Gütermarkt bei gegebenem Zins zu einem Anstieg des Einkommens führen, verschieben die IS-Kurve nach links.</t>
+  </si>
+  <si>
+    <t>Faktoren, die auf Gütermarkt bei gegebenem Zins zu einem Rückgang des Einkommens führen, verschieben die IS-Kurve nach links.</t>
+  </si>
+  <si>
+    <t>Faktoren, die auf Gütermarkt bei gegebenem Zins zu einem Rückgang des Einkommens führen, verschieben die IS-Kurve nach rechts.</t>
+  </si>
+  <si>
+    <t>Bei einer Zinssteuerung können wir die LM-Kurve durch eine horizontale Linie beschreiben.</t>
+  </si>
+  <si>
+    <t>Bei einer Zinssteuerung können wir die LM-Kurve durch eine vertikale Linie beschreiben.</t>
+  </si>
+  <si>
+    <t>Bei einer Zinssteuerung können wir die IS-Kurve durch eine horizontale Linie beschreiben.</t>
+  </si>
+  <si>
+    <t>Das Budgetdefizt wird folgendermaßen berechnet: Steuern - Staatsausgaben</t>
+  </si>
+  <si>
+    <t>Das Budgetdefizt wird folgendermaßen berechnet: Staatsausgaben - Steuern</t>
+  </si>
+  <si>
+    <t>Eine kontraktive Geldpolitik führt zu einer Verschiebung der LM Kurve nach oben.</t>
+  </si>
+  <si>
+    <t>Eine kontraktive Geldpolitik führt zu einer Verschiebung der LM Kurve nach unten.</t>
+  </si>
+  <si>
+    <t>Eine expansive Geldpolitik führt zu einer Verschiebung der LM Kurve nach oben.</t>
+  </si>
+  <si>
+    <t>Eine expansive Geldpolitik führt zu einer Verschiebung der LM Kurve nach unten.</t>
+  </si>
+  <si>
+    <t>Geldpolitik hat einen Einfluss auf die IS Kurve.</t>
+  </si>
+  <si>
+    <t>Geldpolitik hat keinen Einfluss auf die IS Kurve.</t>
+  </si>
+  <si>
+    <t>Fiskalpolitik hat einen Einfluss auf die IS Kurve.</t>
+  </si>
+  <si>
+    <t>Fiskalpolitik hat keinen Einfluss auf die IS Kurve.</t>
+  </si>
+  <si>
+    <t>In the ISLM model, investments decrease as income increases</t>
+  </si>
+  <si>
+    <t>In the ISLM model, investments increase as income increases</t>
+  </si>
+  <si>
+    <t>In the ISLM model, investments decrease as the interest rate increases</t>
+  </si>
+  <si>
+    <t>In the ISLM model, investments increase as the interest rate increases</t>
+  </si>
+  <si>
+    <t>The higher the interest sensitivity of investment demand, the steeper the IS curve</t>
+  </si>
+  <si>
+    <t>The higher the interest sensitivity of investment demand, the flatter the IS curve</t>
+  </si>
+  <si>
+    <t>An increase in the interest rate shifts the goods demand curve downward</t>
+  </si>
+  <si>
+    <t>An increase in the interest rate shifts the goods demand curve upward</t>
+  </si>
+  <si>
+    <t>A reduction in the interest rate shifts the goods demand curve downward</t>
+  </si>
+  <si>
+    <t>A reduction in the interest rate shifts the goods demand curve upward</t>
+  </si>
+  <si>
+    <t>The IS curve has a downward slope</t>
+  </si>
+  <si>
+    <t>The IS curve has an upward slope</t>
+  </si>
+  <si>
+    <t>An increase in government spending shifts the IS curve to the right</t>
+  </si>
+  <si>
+    <t>An increase in government spending shifts the IS curve to the left</t>
+  </si>
+  <si>
+    <t>An increase in taxes shifts the IS curve to the right</t>
+  </si>
+  <si>
+    <t>An increase in taxes shifts the IS curve to the left</t>
+  </si>
+  <si>
+    <t>A decrease in government spending shifts the IS curve to the right</t>
+  </si>
+  <si>
+    <t>A decrease in government spending shifts the IS curve to the left</t>
+  </si>
+  <si>
+    <t>A decrease in taxes shifts the IS curve to the right</t>
+  </si>
+  <si>
+    <t>A decrease in taxes shifts the IS curve to the left</t>
+  </si>
+  <si>
+    <t>The IS curve represents all combinations of interest rates and output where the goods market is in equilibrium</t>
+  </si>
+  <si>
+    <t>Factors in the goods market that lead to a decrease in income at a given interest rate shift the IS curve to the left</t>
+  </si>
+  <si>
+    <t>Factors in the goods market that lead to an increase in income at a given interest rate shift the IS curve to the right</t>
+  </si>
+  <si>
+    <t>Factors in the goods market that lead to an increase in income at a given interest rate shift the IS curve to the left</t>
+  </si>
+  <si>
+    <t>Factors in the goods market that lead to a decrease in income at a given interest rate shift the IS curve to the right</t>
+  </si>
+  <si>
+    <t>Under an interest rate policy, the LM curve can be represented by a horizontal line</t>
+  </si>
+  <si>
+    <t>Under an interest rate policy, the LM curve can be represented by a vertical line</t>
+  </si>
+  <si>
+    <t>Under an interest rate policy, the IS curve can be represented by a horizontal line</t>
+  </si>
+  <si>
+    <t>The budget deficit is calculated as taxes minus government spending</t>
+  </si>
+  <si>
+    <t>The budget deficit is calculated as government spending minus taxes</t>
+  </si>
+  <si>
+    <t>A contractionary monetary policy shifts the LM curve upward</t>
+  </si>
+  <si>
+    <t>A contractionary monetary policy shifts the LM curve downward</t>
+  </si>
+  <si>
+    <t>An expansionary monetary policy shifts the LM curve upward</t>
+  </si>
+  <si>
+    <t>An expansionary monetary policy shifts the LM curve downward</t>
+  </si>
+  <si>
+    <t>Monetary policy influences the IS curve</t>
+  </si>
+  <si>
+    <t>Monetary policy does not influence the IS curve</t>
+  </si>
+  <si>
+    <t>Fiscal policy influences the IS curve</t>
+  </si>
+  <si>
+    <t>Fiscal policy does not influence the IS curve.</t>
   </si>
 </sst>
 </file>
@@ -438,8 +924,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB02651-D15F-5649-AF64-9CB38539F857}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E133" sqref="E133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1379,7 +1868,7 @@
         <v>115</v>
       </c>
       <c r="C56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1390,7 +1879,7 @@
         <v>116</v>
       </c>
       <c r="C57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1401,7 +1890,7 @@
         <v>117</v>
       </c>
       <c r="C58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1412,7 +1901,7 @@
         <v>118</v>
       </c>
       <c r="C59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1434,6 +1923,897 @@
         <v>120</v>
       </c>
       <c r="C61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" t="s">
+        <v>166</v>
+      </c>
+      <c r="C62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" t="s">
+        <v>167</v>
+      </c>
+      <c r="C63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" t="s">
+        <v>168</v>
+      </c>
+      <c r="C64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>124</v>
+      </c>
+      <c r="B65" t="s">
+        <v>169</v>
+      </c>
+      <c r="C65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" t="s">
+        <v>170</v>
+      </c>
+      <c r="C66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>128</v>
+      </c>
+      <c r="B67" t="s">
+        <v>171</v>
+      </c>
+      <c r="C67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>129</v>
+      </c>
+      <c r="B68" t="s">
+        <v>172</v>
+      </c>
+      <c r="C68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>130</v>
+      </c>
+      <c r="B69" t="s">
+        <v>173</v>
+      </c>
+      <c r="C69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>131</v>
+      </c>
+      <c r="B70" t="s">
+        <v>174</v>
+      </c>
+      <c r="C70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>132</v>
+      </c>
+      <c r="B71" t="s">
+        <v>175</v>
+      </c>
+      <c r="C71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>133</v>
+      </c>
+      <c r="B72" t="s">
+        <v>176</v>
+      </c>
+      <c r="C72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>134</v>
+      </c>
+      <c r="B73" t="s">
+        <v>177</v>
+      </c>
+      <c r="C73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>136</v>
+      </c>
+      <c r="B74" t="s">
+        <v>178</v>
+      </c>
+      <c r="C74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>137</v>
+      </c>
+      <c r="B75" t="s">
+        <v>179</v>
+      </c>
+      <c r="C75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>138</v>
+      </c>
+      <c r="B76" t="s">
+        <v>180</v>
+      </c>
+      <c r="C76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>139</v>
+      </c>
+      <c r="B77" t="s">
+        <v>181</v>
+      </c>
+      <c r="C77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>135</v>
+      </c>
+      <c r="B78" t="s">
+        <v>182</v>
+      </c>
+      <c r="C78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>140</v>
+      </c>
+      <c r="B79" t="s">
+        <v>183</v>
+      </c>
+      <c r="C79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>141</v>
+      </c>
+      <c r="B80" t="s">
+        <v>184</v>
+      </c>
+      <c r="C80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>142</v>
+      </c>
+      <c r="B81" t="s">
+        <v>185</v>
+      </c>
+      <c r="C81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>143</v>
+      </c>
+      <c r="B82" t="s">
+        <v>186</v>
+      </c>
+      <c r="C82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>144</v>
+      </c>
+      <c r="B83" t="s">
+        <v>187</v>
+      </c>
+      <c r="C83" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>145</v>
+      </c>
+      <c r="B84" t="s">
+        <v>188</v>
+      </c>
+      <c r="C84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>146</v>
+      </c>
+      <c r="B85" t="s">
+        <v>189</v>
+      </c>
+      <c r="C85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>147</v>
+      </c>
+      <c r="B86" t="s">
+        <v>190</v>
+      </c>
+      <c r="C86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>148</v>
+      </c>
+      <c r="B87" t="s">
+        <v>191</v>
+      </c>
+      <c r="C87" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>151</v>
+      </c>
+      <c r="B88" t="s">
+        <v>192</v>
+      </c>
+      <c r="C88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>149</v>
+      </c>
+      <c r="B89" t="s">
+        <v>193</v>
+      </c>
+      <c r="C89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>150</v>
+      </c>
+      <c r="B90" t="s">
+        <v>194</v>
+      </c>
+      <c r="C90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>152</v>
+      </c>
+      <c r="B91" t="s">
+        <v>195</v>
+      </c>
+      <c r="C91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>153</v>
+      </c>
+      <c r="B92" t="s">
+        <v>196</v>
+      </c>
+      <c r="C92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>154</v>
+      </c>
+      <c r="B93" t="s">
+        <v>197</v>
+      </c>
+      <c r="C93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>155</v>
+      </c>
+      <c r="B94" t="s">
+        <v>198</v>
+      </c>
+      <c r="C94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>156</v>
+      </c>
+      <c r="B95" t="s">
+        <v>199</v>
+      </c>
+      <c r="C95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>160</v>
+      </c>
+      <c r="B96" t="s">
+        <v>200</v>
+      </c>
+      <c r="C96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>157</v>
+      </c>
+      <c r="B97" t="s">
+        <v>201</v>
+      </c>
+      <c r="C97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>161</v>
+      </c>
+      <c r="B98" t="s">
+        <v>202</v>
+      </c>
+      <c r="C98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>158</v>
+      </c>
+      <c r="B99" t="s">
+        <v>203</v>
+      </c>
+      <c r="C99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>162</v>
+      </c>
+      <c r="B100" t="s">
+        <v>204</v>
+      </c>
+      <c r="C100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>159</v>
+      </c>
+      <c r="B101" t="s">
+        <v>205</v>
+      </c>
+      <c r="C101" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>163</v>
+      </c>
+      <c r="B102" t="s">
+        <v>206</v>
+      </c>
+      <c r="C102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>164</v>
+      </c>
+      <c r="B103" t="s">
+        <v>207</v>
+      </c>
+      <c r="C103" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>165</v>
+      </c>
+      <c r="B104" t="s">
+        <v>208</v>
+      </c>
+      <c r="C104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>209</v>
+      </c>
+      <c r="B105" t="s">
+        <v>247</v>
+      </c>
+      <c r="C105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" t="s">
+        <v>248</v>
+      </c>
+      <c r="C106" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>211</v>
+      </c>
+      <c r="B107" t="s">
+        <v>249</v>
+      </c>
+      <c r="C107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>212</v>
+      </c>
+      <c r="B108" t="s">
+        <v>250</v>
+      </c>
+      <c r="C108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>213</v>
+      </c>
+      <c r="B109" t="s">
+        <v>251</v>
+      </c>
+      <c r="C109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>214</v>
+      </c>
+      <c r="B110" t="s">
+        <v>252</v>
+      </c>
+      <c r="C110" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>215</v>
+      </c>
+      <c r="B111" t="s">
+        <v>253</v>
+      </c>
+      <c r="C111" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>216</v>
+      </c>
+      <c r="B112" t="s">
+        <v>254</v>
+      </c>
+      <c r="C112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>217</v>
+      </c>
+      <c r="B113" t="s">
+        <v>255</v>
+      </c>
+      <c r="C113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>218</v>
+      </c>
+      <c r="B114" t="s">
+        <v>256</v>
+      </c>
+      <c r="C114" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>219</v>
+      </c>
+      <c r="B115" t="s">
+        <v>257</v>
+      </c>
+      <c r="C115" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>220</v>
+      </c>
+      <c r="B116" t="s">
+        <v>258</v>
+      </c>
+      <c r="C116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>221</v>
+      </c>
+      <c r="B117" t="s">
+        <v>259</v>
+      </c>
+      <c r="C117" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>222</v>
+      </c>
+      <c r="B118" t="s">
+        <v>260</v>
+      </c>
+      <c r="C118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>223</v>
+      </c>
+      <c r="B119" t="s">
+        <v>261</v>
+      </c>
+      <c r="C119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>224</v>
+      </c>
+      <c r="B120" t="s">
+        <v>262</v>
+      </c>
+      <c r="C120" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>225</v>
+      </c>
+      <c r="B121" t="s">
+        <v>263</v>
+      </c>
+      <c r="C121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>226</v>
+      </c>
+      <c r="B122" t="s">
+        <v>264</v>
+      </c>
+      <c r="C122" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>227</v>
+      </c>
+      <c r="B123" t="s">
+        <v>265</v>
+      </c>
+      <c r="C123" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>228</v>
+      </c>
+      <c r="B124" t="s">
+        <v>266</v>
+      </c>
+      <c r="C124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>229</v>
+      </c>
+      <c r="B125" t="s">
+        <v>267</v>
+      </c>
+      <c r="C125" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B126" t="s">
+        <v>268</v>
+      </c>
+      <c r="C126" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>230</v>
+      </c>
+      <c r="B127" t="s">
+        <v>269</v>
+      </c>
+      <c r="C127" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>231</v>
+      </c>
+      <c r="B128" t="s">
+        <v>270</v>
+      </c>
+      <c r="C128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B129" t="s">
+        <v>271</v>
+      </c>
+      <c r="C129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>234</v>
+      </c>
+      <c r="B130" t="s">
+        <v>272</v>
+      </c>
+      <c r="C130" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>235</v>
+      </c>
+      <c r="B131" t="s">
+        <v>273</v>
+      </c>
+      <c r="C131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>236</v>
+      </c>
+      <c r="B132" t="s">
+        <v>274</v>
+      </c>
+      <c r="C132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>237</v>
+      </c>
+      <c r="B133" t="s">
+        <v>275</v>
+      </c>
+      <c r="C133" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>238</v>
+      </c>
+      <c r="B134" t="s">
+        <v>276</v>
+      </c>
+      <c r="C134" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>239</v>
+      </c>
+      <c r="B135" t="s">
+        <v>277</v>
+      </c>
+      <c r="C135" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>240</v>
+      </c>
+      <c r="B136" t="s">
+        <v>278</v>
+      </c>
+      <c r="C136" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>241</v>
+      </c>
+      <c r="B137" t="s">
+        <v>279</v>
+      </c>
+      <c r="C137" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>242</v>
+      </c>
+      <c r="B138" t="s">
+        <v>280</v>
+      </c>
+      <c r="C138" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>243</v>
+      </c>
+      <c r="B139" t="s">
+        <v>281</v>
+      </c>
+      <c r="C139" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>244</v>
+      </c>
+      <c r="B140" t="s">
+        <v>282</v>
+      </c>
+      <c r="C140" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>245</v>
+      </c>
+      <c r="B141" t="s">
+        <v>283</v>
+      </c>
+      <c r="C141" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>246</v>
+      </c>
+      <c r="B142" t="s">
+        <v>284</v>
+      </c>
+      <c r="C142" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>